<commit_message>
Documentation added for grid generator
</commit_message>
<xml_diff>
--- a/controllers/grid_generator/Timetable template.xlsx
+++ b/controllers/grid_generator/Timetable template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DSSO\Schedule-Source-Grid-Generator\controllers\grid_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB75320-3E3D-4437-AB3D-E85D930E5208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BD1F94-25AB-4DB4-931D-457E4BE8248E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -707,12 +707,12 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1102,8 +1102,8 @@
   </sheetPr>
   <dimension ref="A1:HA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="87" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="CC8" sqref="CC8"/>
+    <sheetView tabSelected="1" zoomScale="48" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="GR6" sqref="GR6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1785,15 +1785,15 @@
       <c r="AI4" s="16"/>
       <c r="AJ4" s="16"/>
       <c r="AK4" s="17"/>
-      <c r="AL4" s="21"/>
-      <c r="AM4" s="22"/>
-      <c r="AN4" s="22"/>
-      <c r="AO4" s="22"/>
-      <c r="AP4" s="22"/>
-      <c r="AQ4" s="22"/>
-      <c r="AR4" s="22"/>
-      <c r="AS4" s="22"/>
-      <c r="AT4" s="22"/>
+      <c r="AL4" s="18"/>
+      <c r="AM4" s="19"/>
+      <c r="AN4" s="19"/>
+      <c r="AO4" s="19"/>
+      <c r="AP4" s="19"/>
+      <c r="AQ4" s="19"/>
+      <c r="AR4" s="19"/>
+      <c r="AS4" s="19"/>
+      <c r="AT4" s="19"/>
       <c r="AU4" s="16"/>
       <c r="AV4" s="16"/>
       <c r="AW4" s="17"/>
@@ -1857,18 +1857,18 @@
       <c r="DC4" s="16"/>
       <c r="DD4" s="16"/>
       <c r="DE4" s="17"/>
-      <c r="DF4" s="21"/>
-      <c r="DG4" s="22"/>
-      <c r="DH4" s="22"/>
-      <c r="DI4" s="22"/>
-      <c r="DJ4" s="22"/>
-      <c r="DK4" s="22"/>
-      <c r="DL4" s="22"/>
-      <c r="DM4" s="22"/>
-      <c r="DN4" s="22"/>
-      <c r="DO4" s="22"/>
-      <c r="DP4" s="22"/>
-      <c r="DQ4" s="23"/>
+      <c r="DF4" s="18"/>
+      <c r="DG4" s="19"/>
+      <c r="DH4" s="19"/>
+      <c r="DI4" s="19"/>
+      <c r="DJ4" s="19"/>
+      <c r="DK4" s="19"/>
+      <c r="DL4" s="19"/>
+      <c r="DM4" s="19"/>
+      <c r="DN4" s="19"/>
+      <c r="DO4" s="19"/>
+      <c r="DP4" s="19"/>
+      <c r="DQ4" s="20"/>
       <c r="DR4" s="15"/>
       <c r="DS4" s="16"/>
       <c r="DT4" s="16"/>
@@ -1893,30 +1893,30 @@
       <c r="EM4" s="16"/>
       <c r="EN4" s="16"/>
       <c r="EO4" s="17"/>
-      <c r="EP4" s="21"/>
-      <c r="EQ4" s="22"/>
-      <c r="ER4" s="22"/>
-      <c r="ES4" s="22"/>
-      <c r="ET4" s="22"/>
-      <c r="EU4" s="22"/>
-      <c r="EV4" s="22"/>
-      <c r="EW4" s="22"/>
-      <c r="EX4" s="22"/>
-      <c r="EY4" s="22"/>
-      <c r="EZ4" s="22"/>
-      <c r="FA4" s="23"/>
-      <c r="FB4" s="21"/>
-      <c r="FC4" s="22"/>
-      <c r="FD4" s="22"/>
-      <c r="FE4" s="22"/>
-      <c r="FF4" s="22"/>
-      <c r="FG4" s="22"/>
-      <c r="FH4" s="22"/>
-      <c r="FI4" s="22"/>
-      <c r="FJ4" s="22"/>
-      <c r="FK4" s="22"/>
-      <c r="FL4" s="22"/>
-      <c r="FM4" s="23"/>
+      <c r="EP4" s="18"/>
+      <c r="EQ4" s="19"/>
+      <c r="ER4" s="19"/>
+      <c r="ES4" s="19"/>
+      <c r="ET4" s="19"/>
+      <c r="EU4" s="19"/>
+      <c r="EV4" s="19"/>
+      <c r="EW4" s="19"/>
+      <c r="EX4" s="19"/>
+      <c r="EY4" s="19"/>
+      <c r="EZ4" s="19"/>
+      <c r="FA4" s="20"/>
+      <c r="FB4" s="18"/>
+      <c r="FC4" s="19"/>
+      <c r="FD4" s="19"/>
+      <c r="FE4" s="19"/>
+      <c r="FF4" s="19"/>
+      <c r="FG4" s="19"/>
+      <c r="FH4" s="19"/>
+      <c r="FI4" s="19"/>
+      <c r="FJ4" s="19"/>
+      <c r="FK4" s="19"/>
+      <c r="FL4" s="19"/>
+      <c r="FM4" s="20"/>
       <c r="FN4" s="15"/>
       <c r="FO4" s="16"/>
       <c r="FP4" s="16"/>
@@ -1962,198 +1962,198 @@
       <c r="A5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="18"/>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="19"/>
-      <c r="AG5" s="19"/>
-      <c r="AH5" s="19"/>
-      <c r="AI5" s="19"/>
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="20"/>
-      <c r="AL5" s="18"/>
-      <c r="AM5" s="19"/>
-      <c r="AN5" s="19"/>
-      <c r="AO5" s="19"/>
-      <c r="AP5" s="19"/>
-      <c r="AQ5" s="19"/>
-      <c r="AR5" s="19"/>
-      <c r="AS5" s="19"/>
-      <c r="AT5" s="19"/>
-      <c r="AU5" s="19"/>
-      <c r="AV5" s="19"/>
-      <c r="AW5" s="20"/>
-      <c r="AX5" s="18"/>
-      <c r="AY5" s="19"/>
-      <c r="AZ5" s="19"/>
-      <c r="BA5" s="19"/>
-      <c r="BB5" s="19"/>
-      <c r="BC5" s="19"/>
-      <c r="BD5" s="19"/>
-      <c r="BE5" s="19"/>
-      <c r="BF5" s="19"/>
-      <c r="BG5" s="19"/>
-      <c r="BH5" s="19"/>
-      <c r="BI5" s="20"/>
-      <c r="BJ5" s="18"/>
-      <c r="BK5" s="19"/>
-      <c r="BL5" s="19"/>
-      <c r="BM5" s="19"/>
-      <c r="BN5" s="19"/>
-      <c r="BO5" s="19"/>
-      <c r="BP5" s="19"/>
-      <c r="BQ5" s="19"/>
-      <c r="BR5" s="19"/>
-      <c r="BS5" s="19"/>
-      <c r="BT5" s="19"/>
-      <c r="BU5" s="20"/>
-      <c r="BV5" s="21"/>
-      <c r="BW5" s="22"/>
-      <c r="BX5" s="22"/>
-      <c r="BY5" s="22"/>
-      <c r="BZ5" s="22"/>
-      <c r="CA5" s="22"/>
-      <c r="CB5" s="22"/>
-      <c r="CC5" s="22"/>
-      <c r="CD5" s="22"/>
-      <c r="CE5" s="22"/>
-      <c r="CF5" s="22"/>
-      <c r="CG5" s="23"/>
-      <c r="CH5" s="18"/>
-      <c r="CI5" s="19"/>
-      <c r="CJ5" s="19"/>
-      <c r="CK5" s="19"/>
-      <c r="CL5" s="19"/>
-      <c r="CM5" s="19"/>
-      <c r="CN5" s="19"/>
-      <c r="CO5" s="19"/>
-      <c r="CP5" s="19"/>
-      <c r="CQ5" s="19"/>
-      <c r="CR5" s="19"/>
-      <c r="CS5" s="20"/>
-      <c r="CT5" s="18"/>
-      <c r="CU5" s="19"/>
-      <c r="CV5" s="19"/>
-      <c r="CW5" s="19"/>
-      <c r="CX5" s="19"/>
-      <c r="CY5" s="22"/>
-      <c r="CZ5" s="22"/>
-      <c r="DA5" s="22"/>
-      <c r="DB5" s="22"/>
-      <c r="DC5" s="22"/>
-      <c r="DD5" s="22"/>
-      <c r="DE5" s="23"/>
-      <c r="DF5" s="21"/>
-      <c r="DG5" s="22"/>
-      <c r="DH5" s="22"/>
-      <c r="DI5" s="22"/>
-      <c r="DJ5" s="22"/>
-      <c r="DK5" s="22"/>
-      <c r="DL5" s="22"/>
-      <c r="DM5" s="19"/>
-      <c r="DN5" s="19"/>
-      <c r="DO5" s="19"/>
-      <c r="DP5" s="19"/>
-      <c r="DQ5" s="20"/>
-      <c r="DR5" s="18"/>
-      <c r="DS5" s="19"/>
-      <c r="DT5" s="22"/>
-      <c r="DU5" s="22"/>
-      <c r="DV5" s="22"/>
-      <c r="DW5" s="22"/>
-      <c r="DX5" s="22"/>
-      <c r="DY5" s="22"/>
-      <c r="DZ5" s="22"/>
-      <c r="EA5" s="22"/>
-      <c r="EB5" s="22"/>
-      <c r="EC5" s="23"/>
-      <c r="ED5" s="18"/>
-      <c r="EE5" s="19"/>
-      <c r="EF5" s="19"/>
-      <c r="EG5" s="19"/>
-      <c r="EH5" s="19"/>
-      <c r="EI5" s="19"/>
-      <c r="EJ5" s="19"/>
-      <c r="EK5" s="19"/>
-      <c r="EL5" s="19"/>
-      <c r="EM5" s="19"/>
-      <c r="EN5" s="19"/>
-      <c r="EO5" s="20"/>
-      <c r="EP5" s="18"/>
-      <c r="EQ5" s="19"/>
-      <c r="ER5" s="19"/>
-      <c r="ES5" s="19"/>
-      <c r="ET5" s="19"/>
-      <c r="EU5" s="19"/>
-      <c r="EV5" s="19"/>
-      <c r="EW5" s="19"/>
-      <c r="EX5" s="19"/>
-      <c r="EY5" s="19"/>
-      <c r="EZ5" s="19"/>
-      <c r="FA5" s="20"/>
-      <c r="FB5" s="18"/>
-      <c r="FC5" s="19"/>
-      <c r="FD5" s="19"/>
-      <c r="FE5" s="19"/>
-      <c r="FF5" s="19"/>
-      <c r="FG5" s="19"/>
-      <c r="FH5" s="19"/>
-      <c r="FI5" s="19"/>
-      <c r="FJ5" s="19"/>
-      <c r="FK5" s="19"/>
-      <c r="FL5" s="19"/>
-      <c r="FM5" s="20"/>
-      <c r="FN5" s="18"/>
-      <c r="FO5" s="19"/>
-      <c r="FP5" s="19"/>
-      <c r="FQ5" s="19"/>
-      <c r="FR5" s="19"/>
-      <c r="FS5" s="19"/>
-      <c r="FT5" s="19"/>
-      <c r="FU5" s="19"/>
-      <c r="FV5" s="19"/>
-      <c r="FW5" s="19"/>
-      <c r="FX5" s="19"/>
-      <c r="FY5" s="20"/>
-      <c r="FZ5" s="18"/>
-      <c r="GA5" s="19"/>
-      <c r="GB5" s="19"/>
-      <c r="GC5" s="19"/>
-      <c r="GD5" s="19"/>
-      <c r="GE5" s="19"/>
-      <c r="GF5" s="19"/>
-      <c r="GG5" s="19"/>
-      <c r="GH5" s="19"/>
-      <c r="GI5" s="19"/>
-      <c r="GJ5" s="19"/>
-      <c r="GK5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="22"/>
+      <c r="AE5" s="22"/>
+      <c r="AF5" s="22"/>
+      <c r="AG5" s="22"/>
+      <c r="AH5" s="22"/>
+      <c r="AI5" s="22"/>
+      <c r="AJ5" s="22"/>
+      <c r="AK5" s="23"/>
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="22"/>
+      <c r="AN5" s="22"/>
+      <c r="AO5" s="22"/>
+      <c r="AP5" s="22"/>
+      <c r="AQ5" s="22"/>
+      <c r="AR5" s="22"/>
+      <c r="AS5" s="22"/>
+      <c r="AT5" s="22"/>
+      <c r="AU5" s="22"/>
+      <c r="AV5" s="22"/>
+      <c r="AW5" s="23"/>
+      <c r="AX5" s="21"/>
+      <c r="AY5" s="22"/>
+      <c r="AZ5" s="22"/>
+      <c r="BA5" s="22"/>
+      <c r="BB5" s="22"/>
+      <c r="BC5" s="22"/>
+      <c r="BD5" s="22"/>
+      <c r="BE5" s="22"/>
+      <c r="BF5" s="22"/>
+      <c r="BG5" s="22"/>
+      <c r="BH5" s="22"/>
+      <c r="BI5" s="23"/>
+      <c r="BJ5" s="21"/>
+      <c r="BK5" s="22"/>
+      <c r="BL5" s="22"/>
+      <c r="BM5" s="22"/>
+      <c r="BN5" s="22"/>
+      <c r="BO5" s="22"/>
+      <c r="BP5" s="22"/>
+      <c r="BQ5" s="22"/>
+      <c r="BR5" s="22"/>
+      <c r="BS5" s="22"/>
+      <c r="BT5" s="22"/>
+      <c r="BU5" s="23"/>
+      <c r="BV5" s="18"/>
+      <c r="BW5" s="19"/>
+      <c r="BX5" s="19"/>
+      <c r="BY5" s="19"/>
+      <c r="BZ5" s="19"/>
+      <c r="CA5" s="19"/>
+      <c r="CB5" s="19"/>
+      <c r="CC5" s="19"/>
+      <c r="CD5" s="19"/>
+      <c r="CE5" s="19"/>
+      <c r="CF5" s="19"/>
+      <c r="CG5" s="20"/>
+      <c r="CH5" s="21"/>
+      <c r="CI5" s="22"/>
+      <c r="CJ5" s="22"/>
+      <c r="CK5" s="22"/>
+      <c r="CL5" s="22"/>
+      <c r="CM5" s="22"/>
+      <c r="CN5" s="22"/>
+      <c r="CO5" s="22"/>
+      <c r="CP5" s="22"/>
+      <c r="CQ5" s="22"/>
+      <c r="CR5" s="22"/>
+      <c r="CS5" s="23"/>
+      <c r="CT5" s="21"/>
+      <c r="CU5" s="22"/>
+      <c r="CV5" s="22"/>
+      <c r="CW5" s="22"/>
+      <c r="CX5" s="22"/>
+      <c r="CY5" s="19"/>
+      <c r="CZ5" s="19"/>
+      <c r="DA5" s="19"/>
+      <c r="DB5" s="19"/>
+      <c r="DC5" s="19"/>
+      <c r="DD5" s="19"/>
+      <c r="DE5" s="20"/>
+      <c r="DF5" s="18"/>
+      <c r="DG5" s="19"/>
+      <c r="DH5" s="19"/>
+      <c r="DI5" s="19"/>
+      <c r="DJ5" s="19"/>
+      <c r="DK5" s="19"/>
+      <c r="DL5" s="19"/>
+      <c r="DM5" s="22"/>
+      <c r="DN5" s="22"/>
+      <c r="DO5" s="22"/>
+      <c r="DP5" s="22"/>
+      <c r="DQ5" s="23"/>
+      <c r="DR5" s="21"/>
+      <c r="DS5" s="22"/>
+      <c r="DT5" s="19"/>
+      <c r="DU5" s="19"/>
+      <c r="DV5" s="19"/>
+      <c r="DW5" s="19"/>
+      <c r="DX5" s="19"/>
+      <c r="DY5" s="19"/>
+      <c r="DZ5" s="19"/>
+      <c r="EA5" s="19"/>
+      <c r="EB5" s="19"/>
+      <c r="EC5" s="20"/>
+      <c r="ED5" s="21"/>
+      <c r="EE5" s="22"/>
+      <c r="EF5" s="22"/>
+      <c r="EG5" s="22"/>
+      <c r="EH5" s="22"/>
+      <c r="EI5" s="22"/>
+      <c r="EJ5" s="22"/>
+      <c r="EK5" s="22"/>
+      <c r="EL5" s="22"/>
+      <c r="EM5" s="22"/>
+      <c r="EN5" s="22"/>
+      <c r="EO5" s="23"/>
+      <c r="EP5" s="21"/>
+      <c r="EQ5" s="22"/>
+      <c r="ER5" s="22"/>
+      <c r="ES5" s="22"/>
+      <c r="ET5" s="22"/>
+      <c r="EU5" s="22"/>
+      <c r="EV5" s="22"/>
+      <c r="EW5" s="22"/>
+      <c r="EX5" s="22"/>
+      <c r="EY5" s="22"/>
+      <c r="EZ5" s="22"/>
+      <c r="FA5" s="23"/>
+      <c r="FB5" s="21"/>
+      <c r="FC5" s="22"/>
+      <c r="FD5" s="22"/>
+      <c r="FE5" s="22"/>
+      <c r="FF5" s="22"/>
+      <c r="FG5" s="22"/>
+      <c r="FH5" s="22"/>
+      <c r="FI5" s="22"/>
+      <c r="FJ5" s="22"/>
+      <c r="FK5" s="22"/>
+      <c r="FL5" s="22"/>
+      <c r="FM5" s="23"/>
+      <c r="FN5" s="21"/>
+      <c r="FO5" s="22"/>
+      <c r="FP5" s="22"/>
+      <c r="FQ5" s="22"/>
+      <c r="FR5" s="22"/>
+      <c r="FS5" s="22"/>
+      <c r="FT5" s="22"/>
+      <c r="FU5" s="22"/>
+      <c r="FV5" s="22"/>
+      <c r="FW5" s="22"/>
+      <c r="FX5" s="22"/>
+      <c r="FY5" s="23"/>
+      <c r="FZ5" s="21"/>
+      <c r="GA5" s="22"/>
+      <c r="GB5" s="22"/>
+      <c r="GC5" s="22"/>
+      <c r="GD5" s="22"/>
+      <c r="GE5" s="22"/>
+      <c r="GF5" s="22"/>
+      <c r="GG5" s="22"/>
+      <c r="GH5" s="22"/>
+      <c r="GI5" s="22"/>
+      <c r="GJ5" s="22"/>
+      <c r="GK5" s="23"/>
       <c r="GL5" s="11"/>
       <c r="GM5" s="11"/>
       <c r="GN5" s="11"/>
@@ -2366,198 +2366,198 @@
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
-      <c r="X7" s="22"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="22"/>
-      <c r="AB7" s="22"/>
-      <c r="AC7" s="22"/>
-      <c r="AD7" s="22"/>
-      <c r="AE7" s="22"/>
-      <c r="AF7" s="22"/>
-      <c r="AG7" s="22"/>
-      <c r="AH7" s="22"/>
-      <c r="AI7" s="22"/>
-      <c r="AJ7" s="22"/>
-      <c r="AK7" s="23"/>
-      <c r="AL7" s="21"/>
-      <c r="AM7" s="22"/>
-      <c r="AN7" s="22"/>
-      <c r="AO7" s="22"/>
-      <c r="AP7" s="22"/>
-      <c r="AQ7" s="22"/>
-      <c r="AR7" s="22"/>
-      <c r="AS7" s="22"/>
-      <c r="AT7" s="22"/>
-      <c r="AU7" s="22"/>
-      <c r="AV7" s="22"/>
-      <c r="AW7" s="23"/>
-      <c r="AX7" s="21"/>
-      <c r="AY7" s="22"/>
-      <c r="AZ7" s="22"/>
-      <c r="BA7" s="22"/>
-      <c r="BB7" s="22"/>
-      <c r="BC7" s="22"/>
-      <c r="BD7" s="22"/>
-      <c r="BE7" s="22"/>
-      <c r="BF7" s="22"/>
-      <c r="BG7" s="22"/>
-      <c r="BH7" s="22"/>
-      <c r="BI7" s="23"/>
-      <c r="BJ7" s="21"/>
-      <c r="BK7" s="22"/>
-      <c r="BL7" s="22"/>
-      <c r="BM7" s="22"/>
-      <c r="BN7" s="22"/>
-      <c r="BO7" s="22"/>
-      <c r="BP7" s="22"/>
-      <c r="BQ7" s="22"/>
-      <c r="BR7" s="22"/>
-      <c r="BS7" s="22"/>
-      <c r="BT7" s="22"/>
-      <c r="BU7" s="23"/>
-      <c r="BV7" s="21"/>
-      <c r="BW7" s="22"/>
-      <c r="BX7" s="22"/>
-      <c r="BY7" s="22"/>
-      <c r="BZ7" s="22"/>
-      <c r="CA7" s="22"/>
-      <c r="CB7" s="22"/>
-      <c r="CC7" s="22"/>
-      <c r="CD7" s="22"/>
-      <c r="CE7" s="22"/>
-      <c r="CF7" s="22"/>
-      <c r="CG7" s="23"/>
-      <c r="CH7" s="21"/>
-      <c r="CI7" s="22"/>
-      <c r="CJ7" s="22"/>
-      <c r="CK7" s="22"/>
-      <c r="CL7" s="22"/>
-      <c r="CM7" s="22"/>
-      <c r="CN7" s="22"/>
-      <c r="CO7" s="22"/>
-      <c r="CP7" s="22"/>
-      <c r="CQ7" s="22"/>
-      <c r="CR7" s="22"/>
-      <c r="CS7" s="23"/>
-      <c r="CT7" s="21"/>
-      <c r="CU7" s="22"/>
-      <c r="CV7" s="22"/>
-      <c r="CW7" s="22"/>
-      <c r="CX7" s="22"/>
-      <c r="CY7" s="22"/>
-      <c r="CZ7" s="22"/>
-      <c r="DA7" s="22"/>
-      <c r="DB7" s="22"/>
-      <c r="DC7" s="22"/>
-      <c r="DD7" s="22"/>
-      <c r="DE7" s="23"/>
-      <c r="DF7" s="21"/>
-      <c r="DG7" s="22"/>
-      <c r="DH7" s="22"/>
-      <c r="DI7" s="22"/>
-      <c r="DJ7" s="22"/>
-      <c r="DK7" s="22"/>
-      <c r="DL7" s="22"/>
-      <c r="DM7" s="22"/>
-      <c r="DN7" s="22"/>
-      <c r="DO7" s="22"/>
-      <c r="DP7" s="22"/>
-      <c r="DQ7" s="23"/>
-      <c r="DR7" s="21"/>
-      <c r="DS7" s="22"/>
-      <c r="DT7" s="22"/>
-      <c r="DU7" s="22"/>
-      <c r="DV7" s="22"/>
-      <c r="DW7" s="22"/>
-      <c r="DX7" s="22"/>
-      <c r="DY7" s="22"/>
-      <c r="DZ7" s="22"/>
-      <c r="EA7" s="22"/>
-      <c r="EB7" s="22"/>
-      <c r="EC7" s="23"/>
-      <c r="ED7" s="21"/>
-      <c r="EE7" s="22"/>
-      <c r="EF7" s="22"/>
-      <c r="EG7" s="22"/>
-      <c r="EH7" s="22"/>
-      <c r="EI7" s="22"/>
-      <c r="EJ7" s="22"/>
-      <c r="EK7" s="22"/>
-      <c r="EL7" s="22"/>
-      <c r="EM7" s="22"/>
-      <c r="EN7" s="22"/>
-      <c r="EO7" s="23"/>
-      <c r="EP7" s="21"/>
-      <c r="EQ7" s="22"/>
-      <c r="ER7" s="22"/>
-      <c r="ES7" s="22"/>
-      <c r="ET7" s="22"/>
-      <c r="EU7" s="22"/>
-      <c r="EV7" s="22"/>
-      <c r="EW7" s="22"/>
-      <c r="EX7" s="22"/>
-      <c r="EY7" s="22"/>
-      <c r="EZ7" s="22"/>
-      <c r="FA7" s="23"/>
-      <c r="FB7" s="21"/>
-      <c r="FC7" s="22"/>
-      <c r="FD7" s="22"/>
-      <c r="FE7" s="22"/>
-      <c r="FF7" s="22"/>
-      <c r="FG7" s="22"/>
-      <c r="FH7" s="22"/>
-      <c r="FI7" s="22"/>
-      <c r="FJ7" s="22"/>
-      <c r="FK7" s="22"/>
-      <c r="FL7" s="22"/>
-      <c r="FM7" s="23"/>
-      <c r="FN7" s="21"/>
-      <c r="FO7" s="22"/>
-      <c r="FP7" s="22"/>
-      <c r="FQ7" s="22"/>
-      <c r="FR7" s="22"/>
-      <c r="FS7" s="22"/>
-      <c r="FT7" s="22"/>
-      <c r="FU7" s="22"/>
-      <c r="FV7" s="22"/>
-      <c r="FW7" s="22"/>
-      <c r="FX7" s="22"/>
-      <c r="FY7" s="23"/>
-      <c r="FZ7" s="21"/>
-      <c r="GA7" s="22"/>
-      <c r="GB7" s="22"/>
-      <c r="GC7" s="22"/>
-      <c r="GD7" s="22"/>
-      <c r="GE7" s="22"/>
-      <c r="GF7" s="22"/>
-      <c r="GG7" s="22"/>
-      <c r="GH7" s="22"/>
-      <c r="GI7" s="22"/>
-      <c r="GJ7" s="22"/>
-      <c r="GK7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="18"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="19"/>
+      <c r="AE7" s="19"/>
+      <c r="AF7" s="19"/>
+      <c r="AG7" s="19"/>
+      <c r="AH7" s="19"/>
+      <c r="AI7" s="19"/>
+      <c r="AJ7" s="19"/>
+      <c r="AK7" s="20"/>
+      <c r="AL7" s="18"/>
+      <c r="AM7" s="19"/>
+      <c r="AN7" s="19"/>
+      <c r="AO7" s="19"/>
+      <c r="AP7" s="19"/>
+      <c r="AQ7" s="19"/>
+      <c r="AR7" s="19"/>
+      <c r="AS7" s="19"/>
+      <c r="AT7" s="19"/>
+      <c r="AU7" s="19"/>
+      <c r="AV7" s="19"/>
+      <c r="AW7" s="20"/>
+      <c r="AX7" s="18"/>
+      <c r="AY7" s="19"/>
+      <c r="AZ7" s="19"/>
+      <c r="BA7" s="19"/>
+      <c r="BB7" s="19"/>
+      <c r="BC7" s="19"/>
+      <c r="BD7" s="19"/>
+      <c r="BE7" s="19"/>
+      <c r="BF7" s="19"/>
+      <c r="BG7" s="19"/>
+      <c r="BH7" s="19"/>
+      <c r="BI7" s="20"/>
+      <c r="BJ7" s="18"/>
+      <c r="BK7" s="19"/>
+      <c r="BL7" s="19"/>
+      <c r="BM7" s="19"/>
+      <c r="BN7" s="19"/>
+      <c r="BO7" s="19"/>
+      <c r="BP7" s="19"/>
+      <c r="BQ7" s="19"/>
+      <c r="BR7" s="19"/>
+      <c r="BS7" s="19"/>
+      <c r="BT7" s="19"/>
+      <c r="BU7" s="20"/>
+      <c r="BV7" s="18"/>
+      <c r="BW7" s="19"/>
+      <c r="BX7" s="19"/>
+      <c r="BY7" s="19"/>
+      <c r="BZ7" s="19"/>
+      <c r="CA7" s="19"/>
+      <c r="CB7" s="19"/>
+      <c r="CC7" s="19"/>
+      <c r="CD7" s="19"/>
+      <c r="CE7" s="19"/>
+      <c r="CF7" s="19"/>
+      <c r="CG7" s="20"/>
+      <c r="CH7" s="18"/>
+      <c r="CI7" s="19"/>
+      <c r="CJ7" s="19"/>
+      <c r="CK7" s="19"/>
+      <c r="CL7" s="19"/>
+      <c r="CM7" s="19"/>
+      <c r="CN7" s="19"/>
+      <c r="CO7" s="19"/>
+      <c r="CP7" s="19"/>
+      <c r="CQ7" s="19"/>
+      <c r="CR7" s="19"/>
+      <c r="CS7" s="20"/>
+      <c r="CT7" s="18"/>
+      <c r="CU7" s="19"/>
+      <c r="CV7" s="19"/>
+      <c r="CW7" s="19"/>
+      <c r="CX7" s="19"/>
+      <c r="CY7" s="19"/>
+      <c r="CZ7" s="19"/>
+      <c r="DA7" s="19"/>
+      <c r="DB7" s="19"/>
+      <c r="DC7" s="19"/>
+      <c r="DD7" s="19"/>
+      <c r="DE7" s="20"/>
+      <c r="DF7" s="18"/>
+      <c r="DG7" s="19"/>
+      <c r="DH7" s="19"/>
+      <c r="DI7" s="19"/>
+      <c r="DJ7" s="19"/>
+      <c r="DK7" s="19"/>
+      <c r="DL7" s="19"/>
+      <c r="DM7" s="19"/>
+      <c r="DN7" s="19"/>
+      <c r="DO7" s="19"/>
+      <c r="DP7" s="19"/>
+      <c r="DQ7" s="20"/>
+      <c r="DR7" s="18"/>
+      <c r="DS7" s="19"/>
+      <c r="DT7" s="19"/>
+      <c r="DU7" s="19"/>
+      <c r="DV7" s="19"/>
+      <c r="DW7" s="19"/>
+      <c r="DX7" s="19"/>
+      <c r="DY7" s="19"/>
+      <c r="DZ7" s="19"/>
+      <c r="EA7" s="19"/>
+      <c r="EB7" s="19"/>
+      <c r="EC7" s="20"/>
+      <c r="ED7" s="18"/>
+      <c r="EE7" s="19"/>
+      <c r="EF7" s="19"/>
+      <c r="EG7" s="19"/>
+      <c r="EH7" s="19"/>
+      <c r="EI7" s="19"/>
+      <c r="EJ7" s="19"/>
+      <c r="EK7" s="19"/>
+      <c r="EL7" s="19"/>
+      <c r="EM7" s="19"/>
+      <c r="EN7" s="19"/>
+      <c r="EO7" s="20"/>
+      <c r="EP7" s="18"/>
+      <c r="EQ7" s="19"/>
+      <c r="ER7" s="19"/>
+      <c r="ES7" s="19"/>
+      <c r="ET7" s="19"/>
+      <c r="EU7" s="19"/>
+      <c r="EV7" s="19"/>
+      <c r="EW7" s="19"/>
+      <c r="EX7" s="19"/>
+      <c r="EY7" s="19"/>
+      <c r="EZ7" s="19"/>
+      <c r="FA7" s="20"/>
+      <c r="FB7" s="18"/>
+      <c r="FC7" s="19"/>
+      <c r="FD7" s="19"/>
+      <c r="FE7" s="19"/>
+      <c r="FF7" s="19"/>
+      <c r="FG7" s="19"/>
+      <c r="FH7" s="19"/>
+      <c r="FI7" s="19"/>
+      <c r="FJ7" s="19"/>
+      <c r="FK7" s="19"/>
+      <c r="FL7" s="19"/>
+      <c r="FM7" s="20"/>
+      <c r="FN7" s="18"/>
+      <c r="FO7" s="19"/>
+      <c r="FP7" s="19"/>
+      <c r="FQ7" s="19"/>
+      <c r="FR7" s="19"/>
+      <c r="FS7" s="19"/>
+      <c r="FT7" s="19"/>
+      <c r="FU7" s="19"/>
+      <c r="FV7" s="19"/>
+      <c r="FW7" s="19"/>
+      <c r="FX7" s="19"/>
+      <c r="FY7" s="20"/>
+      <c r="FZ7" s="18"/>
+      <c r="GA7" s="19"/>
+      <c r="GB7" s="19"/>
+      <c r="GC7" s="19"/>
+      <c r="GD7" s="19"/>
+      <c r="GE7" s="19"/>
+      <c r="GF7" s="19"/>
+      <c r="GG7" s="19"/>
+      <c r="GH7" s="19"/>
+      <c r="GI7" s="19"/>
+      <c r="GJ7" s="19"/>
+      <c r="GK7" s="20"/>
       <c r="GL7" s="11"/>
       <c r="GM7" s="11"/>
       <c r="GN7" s="11"/>
@@ -2595,33 +2595,33 @@
       <c r="Z8" s="15"/>
       <c r="AA8" s="16"/>
       <c r="AB8" s="16"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="22"/>
-      <c r="AE8" s="22"/>
-      <c r="AF8" s="22"/>
-      <c r="AG8" s="22"/>
-      <c r="AH8" s="22"/>
-      <c r="AI8" s="22"/>
-      <c r="AJ8" s="22"/>
-      <c r="AK8" s="23"/>
-      <c r="AL8" s="21"/>
-      <c r="AM8" s="22"/>
-      <c r="AN8" s="22"/>
-      <c r="AO8" s="22"/>
-      <c r="AP8" s="22"/>
-      <c r="AQ8" s="22"/>
-      <c r="AR8" s="22"/>
-      <c r="AS8" s="22"/>
-      <c r="AT8" s="22"/>
-      <c r="AU8" s="22"/>
-      <c r="AV8" s="22"/>
-      <c r="AW8" s="23"/>
-      <c r="AX8" s="21"/>
-      <c r="AY8" s="22"/>
-      <c r="AZ8" s="22"/>
-      <c r="BA8" s="22"/>
-      <c r="BB8" s="22"/>
-      <c r="BC8" s="22"/>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="19"/>
+      <c r="AF8" s="19"/>
+      <c r="AG8" s="19"/>
+      <c r="AH8" s="19"/>
+      <c r="AI8" s="19"/>
+      <c r="AJ8" s="19"/>
+      <c r="AK8" s="20"/>
+      <c r="AL8" s="18"/>
+      <c r="AM8" s="19"/>
+      <c r="AN8" s="19"/>
+      <c r="AO8" s="19"/>
+      <c r="AP8" s="19"/>
+      <c r="AQ8" s="19"/>
+      <c r="AR8" s="19"/>
+      <c r="AS8" s="19"/>
+      <c r="AT8" s="19"/>
+      <c r="AU8" s="19"/>
+      <c r="AV8" s="19"/>
+      <c r="AW8" s="20"/>
+      <c r="AX8" s="18"/>
+      <c r="AY8" s="19"/>
+      <c r="AZ8" s="19"/>
+      <c r="BA8" s="19"/>
+      <c r="BB8" s="19"/>
+      <c r="BC8" s="19"/>
       <c r="BD8" s="16"/>
       <c r="BE8" s="16"/>
       <c r="BF8" s="16"/>
@@ -2655,18 +2655,18 @@
       <c r="CH8" s="15"/>
       <c r="CI8" s="16"/>
       <c r="CJ8" s="16"/>
-      <c r="CK8" s="22"/>
-      <c r="CL8" s="22"/>
-      <c r="CM8" s="22"/>
-      <c r="CN8" s="22"/>
-      <c r="CO8" s="22"/>
-      <c r="CP8" s="22"/>
-      <c r="CQ8" s="22"/>
-      <c r="CR8" s="22"/>
-      <c r="CS8" s="23"/>
-      <c r="CT8" s="21"/>
-      <c r="CU8" s="22"/>
-      <c r="CV8" s="22"/>
+      <c r="CK8" s="19"/>
+      <c r="CL8" s="19"/>
+      <c r="CM8" s="19"/>
+      <c r="CN8" s="19"/>
+      <c r="CO8" s="19"/>
+      <c r="CP8" s="19"/>
+      <c r="CQ8" s="19"/>
+      <c r="CR8" s="19"/>
+      <c r="CS8" s="20"/>
+      <c r="CT8" s="18"/>
+      <c r="CU8" s="19"/>
+      <c r="CV8" s="19"/>
       <c r="CW8" s="16"/>
       <c r="CX8" s="16"/>
       <c r="CY8" s="16"/>

</xml_diff>